<commit_message>
update relazione docx + pdf
</commit_message>
<xml_diff>
--- a/doc/saxpy_mpi_time.xlsx
+++ b/doc/saxpy_mpi_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennycaruso/Desktop/saxpy_mpi/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7A0D56-3AF1-024A-BC88-85E57A9F4335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CBB3EC-B5BE-0C4D-9E26-15EA7FEA1B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{CC9CA06C-A5C2-194D-982B-1612745832FA}"/>
   </bookViews>
@@ -961,7 +961,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
+              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1016,7 +1016,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
+              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1071,7 +1071,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
+              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1119,14 +1119,14 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
+          <c:idx val="1"/>
           <c:order val="3"/>
           <c:tx>
             <c:v>M = 500000</c:v>
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
+              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1169,7 +1169,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-7AD1-9742-BABA-81984F117270}"/>
+              <c16:uniqueId val="{00000000-E95B-9646-943C-1D65C9F20FCC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1538,7 +1538,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$E$2:$E$5</c:f>
+              <c:f>saxpy_mpi_time!$E$20:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1546,13 +1546,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>7.3122500000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.6696699999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0699999999999999E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,7 +1560,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-E6AB-3E4F-A9BE-E90778C0B11A}"/>
+              <c16:uniqueId val="{00000000-AA1D-9D4C-94F5-79510632ABBC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1758,11 +1758,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20</c:f>
+              <c:f>saxpy_mpi_time!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3089,8 +3098,8 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -3197,7 +3206,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -3305,8 +3314,8 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -3413,7 +3422,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -3559,8 +3568,8 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -3667,7 +3676,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -3775,8 +3784,8 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -3883,7 +3892,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11">
@@ -3991,8 +4000,8 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -4099,7 +4108,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12">
@@ -4207,8 +4216,8 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -4315,7 +4324,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="TextBox 13">
@@ -4423,8 +4432,8 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -4531,7 +4540,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="TextBox 14">
@@ -4639,8 +4648,8 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -4747,7 +4756,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="TextBox 15">
@@ -5223,8 +5232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E6F519-5FBC-5F4B-9AEC-F722395A9587}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="82" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update relazione docx + xlsx
</commit_message>
<xml_diff>
--- a/doc/saxpy_mpi_time.xlsx
+++ b/doc/saxpy_mpi_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennycaruso/Desktop/saxpy_mpi/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CBB3EC-B5BE-0C4D-9E26-15EA7FEA1B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409FAD2A-6619-5B47-B34F-B5949843F1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{CC9CA06C-A5C2-194D-982B-1612745832FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{CC9CA06C-A5C2-194D-982B-1612745832FA}"/>
   </bookViews>
   <sheets>
     <sheet name="saxpy_mpi_time" sheetId="1" r:id="rId1"/>
@@ -982,21 +982,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$20:$B$23</c:f>
+              <c:f>saxpy_mpi_time!$D$20:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.7000000000000002E-6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5299999999999998E-5</c:v>
+                  <c:v>0.14624505928853757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.5399999999999998E-5</c:v>
+                  <c:v>6.6787003610108309E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3006599999999999E-2</c:v>
+                  <c:v>8.6033306515744096E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,21 +1037,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$26:$B$29</c:f>
+              <c:f>saxpy_mpi_time!$D$26:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.4E-6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5000000000000003E-5</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.47E-5</c:v>
+                  <c:v>7.2289156626506021E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6788E-2</c:v>
+                  <c:v>8.0852847816973111E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1092,21 +1092,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$32:$B$35</c:f>
+              <c:f>saxpy_mpi_time!$D$32:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.1719999999999999E-4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2209999999999998E-4</c:v>
+                  <c:v>0.62912054494587033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.8929999999999999E-4</c:v>
+                  <c:v>0.58158101877881485</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6771599999999995E-2</c:v>
+                  <c:v>6.7368662369938891E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1147,21 +1147,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$38:$B$41</c:f>
+              <c:f>saxpy_mpi_time!$D$38:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.4074000000000001E-3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2081000000000003E-3</c:v>
+                  <c:v>0.5488635814500411</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9398999999999997E-3</c:v>
+                  <c:v>0.42914898172521065</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5083100000000004E-2</c:v>
+                  <c:v>3.5836021332918258E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1546,13 +1546,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3122500000000007E-2</c:v>
+                  <c:v>7.3122529644268783E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6696699999999998E-2</c:v>
+                  <c:v>1.6696750902527077E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0699999999999999E-5</c:v>
+                  <c:v>1.0754163314468012E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,10 +1604,10 @@
                   <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.80722E-2</c:v>
+                  <c:v>1.8072289156626505E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.01E-5</c:v>
+                  <c:v>1.0106605977121639E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1656,13 +1656,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31456020000000001</c:v>
+                  <c:v>0.31456027247293517</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1453952</c:v>
+                  <c:v>0.14539525469470371</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4210000000000003E-4</c:v>
+                  <c:v>8.4210827962423614E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1711,13 +1711,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2744317</c:v>
+                  <c:v>0.27443179072502055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1072872</c:v>
+                  <c:v>0.10728724543130266</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4795E-3</c:v>
+                  <c:v>4.4795026666147823E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5232,13 +5232,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E6F519-5FBC-5F4B-9AEC-F722395A9587}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="86" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5265,9 +5266,11 @@
         <v>50</v>
       </c>
       <c r="D2" s="2">
+        <f>B2/B2</f>
         <v>1</v>
       </c>
       <c r="E2" s="2">
+        <f>D2/A2</f>
         <v>1</v>
       </c>
     </row>
@@ -5282,9 +5285,11 @@
         <v>500</v>
       </c>
       <c r="D3" s="2">
+        <f>B3/B3</f>
         <v>1</v>
       </c>
       <c r="E3" s="2">
+        <f>D3/A3</f>
         <v>1</v>
       </c>
     </row>
@@ -5299,9 +5304,11 @@
         <v>50000</v>
       </c>
       <c r="D4" s="2">
+        <f>B4/B4</f>
         <v>1</v>
       </c>
       <c r="E4" s="2">
+        <f>D4/A4</f>
         <v>1</v>
       </c>
     </row>
@@ -5316,9 +5323,11 @@
         <v>500000</v>
       </c>
       <c r="D5" s="2">
+        <f>B5/B5</f>
         <v>1</v>
       </c>
       <c r="E5" s="2">
+        <f>D5/A5</f>
         <v>1</v>
       </c>
     </row>
@@ -5333,10 +5342,12 @@
         <v>50</v>
       </c>
       <c r="D6" s="2">
-        <v>0.14624500000000001</v>
+        <f>B2/B6</f>
+        <v>0.14624505928853757</v>
       </c>
       <c r="E6" s="2">
-        <v>7.3122500000000007E-2</v>
+        <f>D6/A6</f>
+        <v>7.3122529644268783E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5350,9 +5361,11 @@
         <v>500</v>
       </c>
       <c r="D7" s="2">
+        <f>B3/B7</f>
         <v>0.12</v>
       </c>
       <c r="E7" s="2">
+        <f>D7/A7</f>
         <v>0.06</v>
       </c>
     </row>
@@ -5367,10 +5380,12 @@
         <v>50000</v>
       </c>
       <c r="D8" s="2">
-        <v>0.62912049999999997</v>
+        <f>B4/B8</f>
+        <v>0.62912054494587033</v>
       </c>
       <c r="E8" s="2">
-        <v>0.31456020000000001</v>
+        <f>D8/A8</f>
+        <v>0.31456027247293517</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5384,10 +5399,12 @@
         <v>500000</v>
       </c>
       <c r="D9" s="2">
-        <v>0.54886349999999995</v>
+        <f>B5/B9</f>
+        <v>0.5488635814500411</v>
       </c>
       <c r="E9" s="2">
-        <v>0.2744317</v>
+        <f>D9/A9</f>
+        <v>0.27443179072502055</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5401,10 +5418,12 @@
         <v>50</v>
       </c>
       <c r="D10" s="2">
-        <v>6.6786999999999999E-2</v>
+        <f>B2/B10</f>
+        <v>6.6787003610108309E-2</v>
       </c>
       <c r="E10" s="2">
-        <v>1.6696699999999998E-2</v>
+        <f>D10/A10</f>
+        <v>1.6696750902527077E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5418,10 +5437,12 @@
         <v>500</v>
       </c>
       <c r="D11" s="2">
-        <v>7.2289099999999995E-2</v>
+        <f>B3/B11</f>
+        <v>7.2289156626506021E-2</v>
       </c>
       <c r="E11" s="2">
-        <v>1.80722E-2</v>
+        <f>D11/A11</f>
+        <v>1.8072289156626505E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5435,10 +5456,12 @@
         <v>50000</v>
       </c>
       <c r="D12" s="2">
-        <v>0.58158100000000001</v>
+        <f>B4/B12</f>
+        <v>0.58158101877881485</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1453952</v>
+        <f>D12/A12</f>
+        <v>0.14539525469470371</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5452,10 +5475,12 @@
         <v>500000</v>
       </c>
       <c r="D13" s="2">
-        <v>0.4291489</v>
+        <f>B5/B13</f>
+        <v>0.42914898172521065</v>
       </c>
       <c r="E13" s="2">
-        <v>0.1072872</v>
+        <f>D13/A13</f>
+        <v>0.10728724543130266</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5469,10 +5494,12 @@
         <v>50</v>
       </c>
       <c r="D14" s="2">
-        <v>8.6000000000000003E-5</v>
+        <f>B2/B14</f>
+        <v>8.6033306515744096E-5</v>
       </c>
       <c r="E14" s="2">
-        <v>1.0699999999999999E-5</v>
+        <f>D14/A14</f>
+        <v>1.0754163314468012E-5</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5486,10 +5513,12 @@
         <v>500</v>
       </c>
       <c r="D15" s="2">
-        <v>8.0799999999999999E-5</v>
+        <f>B3/B15</f>
+        <v>8.0852847816973111E-5</v>
       </c>
       <c r="E15" s="2">
-        <v>1.01E-5</v>
+        <f>D15/A15</f>
+        <v>1.0106605977121639E-5</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5503,10 +5532,12 @@
         <v>50000</v>
       </c>
       <c r="D16" s="2">
-        <v>6.7368000000000003E-3</v>
+        <f>B4/B16</f>
+        <v>6.7368662369938891E-3</v>
       </c>
       <c r="E16" s="2">
-        <v>8.4210000000000003E-4</v>
+        <f>D16/A16</f>
+        <v>8.4210827962423614E-4</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5520,10 +5551,12 @@
         <v>500000</v>
       </c>
       <c r="D17" s="2">
-        <v>3.5836E-2</v>
+        <f>B5/B17</f>
+        <v>3.5836021332918258E-2</v>
       </c>
       <c r="E17" s="2">
-        <v>4.4795E-3</v>
+        <f>D17/A17</f>
+        <v>4.4795026666147823E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5550,9 +5583,11 @@
         <v>50</v>
       </c>
       <c r="D20" s="2">
+        <f>B20/B20</f>
         <v>1</v>
       </c>
       <c r="E20" s="2">
+        <f>D20/A20</f>
         <v>1</v>
       </c>
     </row>
@@ -5567,10 +5602,12 @@
         <v>50</v>
       </c>
       <c r="D21" s="2">
-        <v>0.14624500000000001</v>
+        <f>B20/B21</f>
+        <v>0.14624505928853757</v>
       </c>
       <c r="E21" s="2">
-        <v>7.3122500000000007E-2</v>
+        <f>D21/A21</f>
+        <v>7.3122529644268783E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5584,10 +5621,12 @@
         <v>50</v>
       </c>
       <c r="D22" s="2">
-        <v>6.6786999999999999E-2</v>
+        <f>B20/B22</f>
+        <v>6.6787003610108309E-2</v>
       </c>
       <c r="E22" s="2">
-        <v>1.6696699999999998E-2</v>
+        <f>D22/A22</f>
+        <v>1.6696750902527077E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5601,10 +5640,12 @@
         <v>50</v>
       </c>
       <c r="D23" s="2">
-        <v>8.6000000000000003E-5</v>
+        <f>B20/B23</f>
+        <v>8.6033306515744096E-5</v>
       </c>
       <c r="E23" s="2">
-        <v>1.0699999999999999E-5</v>
+        <f>D23/A23</f>
+        <v>1.0754163314468012E-5</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5631,9 +5672,11 @@
         <v>500</v>
       </c>
       <c r="D26" s="2">
+        <f>B26/B26</f>
         <v>1</v>
       </c>
       <c r="E26" s="2">
+        <f>D26/A26</f>
         <v>1</v>
       </c>
     </row>
@@ -5648,9 +5691,11 @@
         <v>500</v>
       </c>
       <c r="D27" s="2">
+        <f>B26/B27</f>
         <v>0.12</v>
       </c>
       <c r="E27" s="2">
+        <f>D27/A27</f>
         <v>0.06</v>
       </c>
     </row>
@@ -5665,10 +5710,12 @@
         <v>500</v>
       </c>
       <c r="D28" s="2">
-        <v>7.2289099999999995E-2</v>
+        <f>B26/B28</f>
+        <v>7.2289156626506021E-2</v>
       </c>
       <c r="E28" s="2">
-        <v>1.80722E-2</v>
+        <f>D28/A28</f>
+        <v>1.8072289156626505E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5682,10 +5729,12 @@
         <v>500</v>
       </c>
       <c r="D29" s="2">
-        <v>8.0799999999999999E-5</v>
+        <f>B26/B29</f>
+        <v>8.0852847816973111E-5</v>
       </c>
       <c r="E29" s="2">
-        <v>1.01E-5</v>
+        <f>D29/A29</f>
+        <v>1.0106605977121639E-5</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5712,9 +5761,11 @@
         <v>50000</v>
       </c>
       <c r="D32" s="2">
+        <f>B32/B32</f>
         <v>1</v>
       </c>
       <c r="E32" s="2">
+        <f>D32/A32</f>
         <v>1</v>
       </c>
     </row>
@@ -5729,10 +5780,12 @@
         <v>50000</v>
       </c>
       <c r="D33" s="2">
-        <v>0.62912049999999997</v>
+        <f>B32/B33</f>
+        <v>0.62912054494587033</v>
       </c>
       <c r="E33" s="2">
-        <v>0.31456020000000001</v>
+        <f>D33/A33</f>
+        <v>0.31456027247293517</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5746,10 +5799,12 @@
         <v>50000</v>
       </c>
       <c r="D34" s="2">
-        <v>0.58158100000000001</v>
+        <f>B32/B34</f>
+        <v>0.58158101877881485</v>
       </c>
       <c r="E34" s="2">
-        <v>0.1453952</v>
+        <f>D34/A34</f>
+        <v>0.14539525469470371</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5763,10 +5818,12 @@
         <v>50000</v>
       </c>
       <c r="D35" s="2">
-        <v>6.7368000000000003E-3</v>
+        <f>B32/B35</f>
+        <v>6.7368662369938891E-3</v>
       </c>
       <c r="E35" s="2">
-        <v>8.4210000000000003E-4</v>
+        <f>D35/A35</f>
+        <v>8.4210827962423614E-4</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5793,9 +5850,11 @@
         <v>500000</v>
       </c>
       <c r="D38" s="2">
+        <f>B38/B38</f>
         <v>1</v>
       </c>
       <c r="E38" s="2">
+        <f>D38/A38</f>
         <v>1</v>
       </c>
     </row>
@@ -5810,10 +5869,12 @@
         <v>500000</v>
       </c>
       <c r="D39" s="2">
-        <v>0.54886349999999995</v>
+        <f>B38/B39</f>
+        <v>0.5488635814500411</v>
       </c>
       <c r="E39" s="2">
-        <v>0.2744317</v>
+        <f>D39/A39</f>
+        <v>0.27443179072502055</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5827,10 +5888,12 @@
         <v>500000</v>
       </c>
       <c r="D40" s="2">
-        <v>0.4291489</v>
+        <f>B38/B40</f>
+        <v>0.42914898172521065</v>
       </c>
       <c r="E40" s="2">
-        <v>0.1072872</v>
+        <f>D40/A40</f>
+        <v>0.10728724543130266</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -5844,10 +5907,12 @@
         <v>500000</v>
       </c>
       <c r="D41" s="2">
-        <v>3.5836E-2</v>
+        <f>B38/B41</f>
+        <v>3.5836021332918258E-2</v>
       </c>
       <c r="E41" s="2">
-        <v>4.4795E-3</v>
+        <f>D41/A41</f>
+        <v>4.4795026666147823E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added other time results only in xlsx
</commit_message>
<xml_diff>
--- a/doc/saxpy_mpi_time.xlsx
+++ b/doc/saxpy_mpi_time.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennycaruso/Desktop/saxpy_mpi/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409FAD2A-6619-5B47-B34F-B5949843F1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B87E663-4758-C143-AF86-4BFAF45ED3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{CC9CA06C-A5C2-194D-982B-1612745832FA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{379D3EE4-06AA-004F-B154-DB2AAE66E474}"/>
   </bookViews>
   <sheets>
-    <sheet name="saxpy_mpi_time" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -269,7 +272,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -290,7 +293,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$20:$B$23</c:f>
+              <c:f>[1]saxpy_mpi_time!$H$2:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -312,7 +315,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-77ED-6141-AA08-E8F4CEDCEDA1}"/>
+              <c16:uniqueId val="{00000000-D971-004C-8ADA-8C23166DFBE4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -348,7 +351,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -369,7 +372,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$26:$B$29</c:f>
+              <c:f>[1]saxpy_mpi_time!$H$8:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -391,7 +394,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-77ED-6141-AA08-E8F4CEDCEDA1}"/>
+              <c16:uniqueId val="{00000001-D971-004C-8ADA-8C23166DFBE4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -427,7 +430,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -448,7 +451,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$32:$B$35</c:f>
+              <c:f>[1]saxpy_mpi_time!$H$38:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -470,7 +473,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-77ED-6141-AA08-E8F4CEDCEDA1}"/>
+              <c16:uniqueId val="{00000002-D971-004C-8ADA-8C23166DFBE4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -506,7 +509,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -527,7 +530,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$B$38:$B$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$H$44:$H$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -549,7 +552,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-77ED-6141-AA08-E8F4CEDCEDA1}"/>
+              <c16:uniqueId val="{00000003-D971-004C-8ADA-8C23166DFBE4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -928,6 +931,1490 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Efficienza e Numero</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> di processori</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>M = 50</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$2:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3122529644268783E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6696750902527077E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0754163314468012E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>M = 500</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$8:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8072289156626505E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0106605977121639E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>M = 50000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$38:$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31456027247293517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14539525469470371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4210827962423614E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>M = 500000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$44:$K$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27443179072502055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10728724543130266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4795026666147823E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Efficienza Ideale</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>M = 50</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$2:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3122529644268783E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6696750902527077E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0754163314468012E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>M = 500</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$8:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8072289156626505E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0106605977121639E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>M = 50000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$38:$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31456027247293517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14539525469470371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4210827962423614E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>M = 500000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$44:$K$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27443179072502055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10728724543130266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4795026666147823E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Efficienza Ideale</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>M = 50</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$2:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3122529644268783E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6696750902527077E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0754163314468012E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>M = 500</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$8:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8072289156626505E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0106605977121639E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>M = 50000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$38:$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31456027247293517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14539525469470371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4210827962423614E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:v>M = 500000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$44:$K$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27443179072502055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10728724543130266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4795026666147823E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:v>Efficienza Ideale</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:v>M = 50</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$2:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3122529644268783E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6696750902527077E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0754163314468012E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:v>M = 500</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$8:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8072289156626505E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0106605977121639E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:v>M = 50000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$38:$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31456027247293517</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14539525469470371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4210827962423614E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:v>M = 500000</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$K$44:$K$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27443179072502055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10728724543130266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4795026666147823E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:v>Efficienza Ideale</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]saxpy_mpi_time!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-C940-6E40-84E5-17911AFA92E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1305355200"/>
+        <c:axId val="1282646304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1305355200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Numero</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Processori</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1282646304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1282646304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficienza</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1305355200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Speed-up e Numero</a:t>
             </a:r>
             <a:r>
@@ -961,7 +2448,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -982,7 +2469,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$D$20:$D$23</c:f>
+              <c:f>[1]saxpy_mpi_time!$J$2:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1004,7 +2491,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-7AD1-9742-BABA-81984F117270}"/>
+              <c16:uniqueId val="{00000000-CAAD-B643-B70E-C93D68D966A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1016,7 +2503,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1037,7 +2524,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$D$26:$D$29</c:f>
+              <c:f>[1]saxpy_mpi_time!$J$8:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1059,7 +2546,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-7AD1-9742-BABA-81984F117270}"/>
+              <c16:uniqueId val="{00000001-CAAD-B643-B70E-C93D68D966A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1071,7 +2558,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1092,7 +2579,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$D$32:$D$35</c:f>
+              <c:f>[1]saxpy_mpi_time!$J$38:$J$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1114,7 +2601,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-7AD1-9742-BABA-81984F117270}"/>
+              <c16:uniqueId val="{00000002-CAAD-B643-B70E-C93D68D966A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1126,7 +2613,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$A$38:$A$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$G$44:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1147,7 +2634,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>saxpy_mpi_time!$D$38:$D$41</c:f>
+              <c:f>[1]saxpy_mpi_time!$J$44:$J$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1169,7 +2656,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E95B-9646-943C-1D65C9F20FCC}"/>
+              <c16:uniqueId val="{00000003-CAAD-B643-B70E-C93D68D966A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1334,617 +2821,6 @@
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>Speed-up</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1305355200"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-IT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Efficienza e Numero</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> di processori</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>M = 50</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$E$20:$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.3122529644268783E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6696750902527077E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0754163314468012E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AA1D-9D4C-94F5-79510632ABBC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>M = 500</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$E$26:$E$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8072289156626505E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0106605977121639E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-E6AB-3E4F-A9BE-E90778C0B11A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>M = 50000</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$E$32:$E$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.31456027247293517</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.14539525469470371</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.4210827962423614E-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-E6AB-3E4F-A9BE-E90778C0B11A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>M = 500000</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$E$38:$E$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27443179072502055</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.10728724543130266</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.4795026666147823E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-E6AB-3E4F-A9BE-E90778C0B11A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>Efficienza Ideale</c:v>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$A$20:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>saxpy_mpi_time!$A$2:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-E6AB-3E4F-A9BE-E90778C0B11A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1305355200"/>
-        <c:axId val="1282646304"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1305355200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Numero</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Processori</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1282646304"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1282646304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Efficienza</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2607,75 +3483,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>108601</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>10908</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="65" cy="172227"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C076613D-0E34-3A41-B785-3B8A6FC3E61F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6686550" y="3063793"/>
-          <a:ext cx="65" cy="172227"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>25358</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2">
+            <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DB601A2-90F5-0133-3D71-20FF20ABF489}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8F629D-8CDC-A64C-AA86-97363472F8F4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2683,7 +3504,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2498866" y="5967"/>
+              <a:off x="2628858" y="5967"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2776,13 +3597,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2">
+            <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DB601A2-90F5-0133-3D71-20FF20ABF489}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8F629D-8CDC-A64C-AA86-97363472F8F4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2790,7 +3611,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2498866" y="5967"/>
+              <a:off x="2628858" y="5967"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2818,6 +3639,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="it-IT" sz="1400" b="0" i="0">
                   <a:solidFill>
@@ -2883,14 +3705,14 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3">
+            <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EE91748-E345-4E41-926D-46ABD8E502E9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{265CBEB5-A28F-724B-84DF-DC4644A85AA6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2898,7 +3720,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3338309" y="5861"/>
+              <a:off x="3719635" y="5861"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2991,13 +3813,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3">
+            <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EE91748-E345-4E41-926D-46ABD8E502E9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{265CBEB5-A28F-724B-84DF-DC4644A85AA6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3005,7 +3827,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3338309" y="5861"/>
+              <a:off x="3719635" y="5861"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3033,6 +3855,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="it-IT" sz="1400" b="0" i="0">
                   <a:solidFill>
@@ -3098,14 +3921,14 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="TextBox 5">
+            <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE724E1-30B7-5C48-A224-119A7D419304}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC06D71B-6AE4-C541-AC17-25845663215B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3113,7 +3936,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2514558" y="5967"/>
+              <a:off x="2628858" y="4311267"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3206,13 +4029,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="TextBox 5">
+            <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE724E1-30B7-5C48-A224-119A7D419304}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC06D71B-6AE4-C541-AC17-25845663215B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3220,7 +4043,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2514558" y="5967"/>
+              <a:off x="2628858" y="4311267"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3314,14 +4137,14 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
+            <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC5E512-8862-084E-8A5D-FCA8C2CA109B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3B70ABC-BE15-F346-A169-2A470D43B59F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3329,7 +4152,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3368268" y="5861"/>
+              <a:off x="3719635" y="4311161"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3422,13 +4245,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
+            <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC5E512-8862-084E-8A5D-FCA8C2CA109B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3B70ABC-BE15-F346-A169-2A470D43B59F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3436,7 +4259,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3368268" y="5861"/>
+              <a:off x="3719635" y="4311161"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3522,44 +4345,6 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>186266</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>445647</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>51278</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1A37A78-E864-31F3-17B2-99DA6AF59657}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -3568,14 +4353,14 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="TextBox 10">
+            <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33927EA-97E4-0C4A-B8AF-797387007290}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E494F213-C202-2D41-BEF0-F53C0DB28978}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3583,7 +4368,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2622651" y="4264764"/>
+              <a:off x="2628858" y="5720967"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3676,13 +4461,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="TextBox 10">
+            <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33927EA-97E4-0C4A-B8AF-797387007290}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E494F213-C202-2D41-BEF0-F53C0DB28978}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3690,7 +4475,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2622651" y="4264764"/>
+              <a:off x="2628858" y="5720967"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3784,14 +4569,14 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="TextBox 11">
+            <xdr:cNvPr id="17" name="TextBox 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{269815BD-8079-B246-BC9B-943B435799F7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A8E6FE-8523-6447-AA23-682E122ED045}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3799,7 +4584,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3467831" y="4264658"/>
+              <a:off x="3719635" y="5720861"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3892,13 +4677,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="12" name="TextBox 11">
+            <xdr:cNvPr id="17" name="TextBox 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{269815BD-8079-B246-BC9B-943B435799F7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A8E6FE-8523-6447-AA23-682E122ED045}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3906,7 +4691,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3467831" y="4264658"/>
+              <a:off x="3719635" y="5720861"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4000,14 +4785,14 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="TextBox 12">
+            <xdr:cNvPr id="18" name="TextBox 17">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9A2B278-1303-C849-8AD8-23D252E8A663}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F007F6-D63C-9D4E-AED2-9E897BFC016F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4015,7 +4800,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2622651" y="5658899"/>
+              <a:off x="2628858" y="7130667"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4108,13 +4893,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="13" name="TextBox 12">
+            <xdr:cNvPr id="18" name="TextBox 17">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9A2B278-1303-C849-8AD8-23D252E8A663}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F007F6-D63C-9D4E-AED2-9E897BFC016F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4122,7 +4907,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2622651" y="5658899"/>
+              <a:off x="2628858" y="7130667"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4216,14 +5001,14 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
+            <xdr:cNvPr id="19" name="TextBox 18">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B55E9C-D539-BD41-A5D8-2CC3F5A55481}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4998887C-62AA-3942-AD64-124431F65E5F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4231,7 +5016,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3467831" y="5658793"/>
+              <a:off x="3719635" y="7130561"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4324,13 +5109,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
+            <xdr:cNvPr id="19" name="TextBox 18">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B55E9C-D539-BD41-A5D8-2CC3F5A55481}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4998887C-62AA-3942-AD64-124431F65E5F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4338,7 +5123,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3467831" y="5658793"/>
+              <a:off x="3719635" y="7130561"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4432,14 +5217,14 @@
       <xdr:rowOff>5967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242182" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
+            <xdr:cNvPr id="20" name="TextBox 19">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF5DFF0C-DA6F-B846-B93D-76B18FCAD4C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6A32E3-7CF3-2E4C-95E0-24F1BBD98694}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4447,7 +5232,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2622651" y="7053035"/>
+              <a:off x="2628858" y="8540367"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4540,13 +5325,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="TextBox 14">
+            <xdr:cNvPr id="20" name="TextBox 19">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF5DFF0C-DA6F-B846-B93D-76B18FCAD4C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6A32E3-7CF3-2E4C-95E0-24F1BBD98694}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4554,7 +5339,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2622651" y="7053035"/>
+              <a:off x="2628858" y="8540367"/>
               <a:ext cx="242182" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4648,14 +5433,14 @@
       <xdr:rowOff>5861</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257571" cy="219099"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextBox 15">
+            <xdr:cNvPr id="21" name="TextBox 20">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7863E7C8-4418-334F-9C0D-ACD7FA83D060}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF2EA340-AB25-1C4A-B38A-958323057654}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4663,7 +5448,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3467831" y="7052929"/>
+              <a:off x="3719635" y="8540261"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4756,13 +5541,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextBox 15">
+            <xdr:cNvPr id="21" name="TextBox 20">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7863E7C8-4418-334F-9C0D-ACD7FA83D060}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF2EA340-AB25-1C4A-B38A-958323057654}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4770,7 +5555,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3467831" y="7052929"/>
+              <a:off x="3719635" y="8540261"/>
               <a:ext cx="257571" cy="219099"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -4858,27 +5643,67 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>211666</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>86431</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>360795</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>135466</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>458937</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>208503</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="17" name="Chart 16">
+        <xdr:cNvPr id="22" name="Chart 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44BB9F4C-915A-583D-BBEA-B719178C55F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{452BB987-E7EC-894A-B708-E96861278B66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>22720</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>186010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B83F8D-055F-9A44-84A6-B6C7EE73F274}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4894,23 +5719,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>250729</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>204321</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>289419</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>147977</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="Chart 17">
+        <xdr:cNvPr id="24" name="Chart 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDAA802B-BEDD-3F41-8E82-2C1161751EDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC26E77-6F0C-0F40-AC40-951FD4CA15EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4931,6 +5756,248 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="saxpy_mpi_time"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+          <cell r="G2">
+            <v>1</v>
+          </cell>
+          <cell r="H2">
+            <v>3.7000000000000002E-6</v>
+          </cell>
+          <cell r="J2">
+            <v>1</v>
+          </cell>
+          <cell r="K2">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>1</v>
+          </cell>
+          <cell r="G3">
+            <v>2</v>
+          </cell>
+          <cell r="H3">
+            <v>2.5299999999999998E-5</v>
+          </cell>
+          <cell r="J3">
+            <v>0.14624505928853757</v>
+          </cell>
+          <cell r="K3">
+            <v>7.3122529644268783E-2</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>1</v>
+          </cell>
+          <cell r="G4">
+            <v>4</v>
+          </cell>
+          <cell r="H4">
+            <v>5.5399999999999998E-5</v>
+          </cell>
+          <cell r="J4">
+            <v>6.6787003610108309E-2</v>
+          </cell>
+          <cell r="K4">
+            <v>1.6696750902527077E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>1</v>
+          </cell>
+          <cell r="G5">
+            <v>8</v>
+          </cell>
+          <cell r="H5">
+            <v>4.3006599999999999E-2</v>
+          </cell>
+          <cell r="J5">
+            <v>8.6033306515744096E-5</v>
+          </cell>
+          <cell r="K5">
+            <v>1.0754163314468012E-5</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>1</v>
+          </cell>
+          <cell r="H8">
+            <v>5.4E-6</v>
+          </cell>
+          <cell r="J8">
+            <v>1</v>
+          </cell>
+          <cell r="K8">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1</v>
+          </cell>
+          <cell r="H9">
+            <v>4.5000000000000003E-5</v>
+          </cell>
+          <cell r="J9">
+            <v>0.12</v>
+          </cell>
+          <cell r="K9">
+            <v>0.06</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="H10">
+            <v>7.47E-5</v>
+          </cell>
+          <cell r="J10">
+            <v>7.2289156626506021E-2</v>
+          </cell>
+          <cell r="K10">
+            <v>1.8072289156626505E-2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="H11">
+            <v>6.6788E-2</v>
+          </cell>
+          <cell r="J11">
+            <v>8.0852847816973111E-5</v>
+          </cell>
+          <cell r="K11">
+            <v>1.0106605977121639E-5</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="H38">
+            <v>5.1719999999999999E-4</v>
+          </cell>
+          <cell r="J38">
+            <v>1</v>
+          </cell>
+          <cell r="K38">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="H39">
+            <v>8.2209999999999998E-4</v>
+          </cell>
+          <cell r="J39">
+            <v>0.62912054494587033</v>
+          </cell>
+          <cell r="K39">
+            <v>0.31456027247293517</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="H40">
+            <v>8.8929999999999999E-4</v>
+          </cell>
+          <cell r="J40">
+            <v>0.58158101877881485</v>
+          </cell>
+          <cell r="K40">
+            <v>0.14539525469470371</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="H41">
+            <v>7.6771599999999995E-2</v>
+          </cell>
+          <cell r="J41">
+            <v>6.7368662369938891E-3</v>
+          </cell>
+          <cell r="K41">
+            <v>8.4210827962423614E-4</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="G44">
+            <v>1</v>
+          </cell>
+          <cell r="H44">
+            <v>3.4074000000000001E-3</v>
+          </cell>
+          <cell r="J44">
+            <v>1</v>
+          </cell>
+          <cell r="K44">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="G45">
+            <v>2</v>
+          </cell>
+          <cell r="H45">
+            <v>6.2081000000000003E-3</v>
+          </cell>
+          <cell r="J45">
+            <v>0.5488635814500411</v>
+          </cell>
+          <cell r="K45">
+            <v>0.27443179072502055</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="G46">
+            <v>4</v>
+          </cell>
+          <cell r="H46">
+            <v>7.9398999999999997E-3</v>
+          </cell>
+          <cell r="J46">
+            <v>0.42914898172521065</v>
+          </cell>
+          <cell r="K46">
+            <v>0.10728724543130266</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="G47">
+            <v>8</v>
+          </cell>
+          <cell r="H47">
+            <v>9.5083100000000004E-2</v>
+          </cell>
+          <cell r="J47">
+            <v>3.5836021332918258E-2</v>
+          </cell>
+          <cell r="K47">
+            <v>4.4795026666147823E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5229,18 +6296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E6F519-5FBC-5F4B-9AEC-F722395A9587}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F577B2EF-101D-A349-AD5B-C4341ACDEBC4}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="86" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -5270,7 +6333,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <f>D2/A2</f>
+        <f t="shared" ref="E2:E17" si="0">D2/A2</f>
         <v>1</v>
       </c>
     </row>
@@ -5289,7 +6352,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <f>D3/A3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5308,7 +6371,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f>D4/A4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5327,7 +6390,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f>D5/A5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -5346,7 +6409,7 @@
         <v>0.14624505928853757</v>
       </c>
       <c r="E6" s="2">
-        <f>D6/A6</f>
+        <f t="shared" si="0"/>
         <v>7.3122529644268783E-2</v>
       </c>
     </row>
@@ -5365,7 +6428,7 @@
         <v>0.12</v>
       </c>
       <c r="E7" s="2">
-        <f>D7/A7</f>
+        <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
     </row>
@@ -5384,7 +6447,7 @@
         <v>0.62912054494587033</v>
       </c>
       <c r="E8" s="2">
-        <f>D8/A8</f>
+        <f t="shared" si="0"/>
         <v>0.31456027247293517</v>
       </c>
     </row>
@@ -5403,7 +6466,7 @@
         <v>0.5488635814500411</v>
       </c>
       <c r="E9" s="2">
-        <f>D9/A9</f>
+        <f t="shared" si="0"/>
         <v>0.27443179072502055</v>
       </c>
     </row>
@@ -5422,7 +6485,7 @@
         <v>6.6787003610108309E-2</v>
       </c>
       <c r="E10" s="2">
-        <f>D10/A10</f>
+        <f t="shared" si="0"/>
         <v>1.6696750902527077E-2</v>
       </c>
     </row>
@@ -5441,7 +6504,7 @@
         <v>7.2289156626506021E-2</v>
       </c>
       <c r="E11" s="2">
-        <f>D11/A11</f>
+        <f t="shared" si="0"/>
         <v>1.8072289156626505E-2</v>
       </c>
     </row>
@@ -5460,7 +6523,7 @@
         <v>0.58158101877881485</v>
       </c>
       <c r="E12" s="2">
-        <f>D12/A12</f>
+        <f t="shared" si="0"/>
         <v>0.14539525469470371</v>
       </c>
     </row>
@@ -5479,7 +6542,7 @@
         <v>0.42914898172521065</v>
       </c>
       <c r="E13" s="2">
-        <f>D13/A13</f>
+        <f t="shared" si="0"/>
         <v>0.10728724543130266</v>
       </c>
     </row>
@@ -5498,7 +6561,7 @@
         <v>8.6033306515744096E-5</v>
       </c>
       <c r="E14" s="2">
-        <f>D14/A14</f>
+        <f t="shared" si="0"/>
         <v>1.0754163314468012E-5</v>
       </c>
     </row>
@@ -5517,7 +6580,7 @@
         <v>8.0852847816973111E-5</v>
       </c>
       <c r="E15" s="2">
-        <f>D15/A15</f>
+        <f t="shared" si="0"/>
         <v>1.0106605977121639E-5</v>
       </c>
     </row>
@@ -5536,7 +6599,7 @@
         <v>6.7368662369938891E-3</v>
       </c>
       <c r="E16" s="2">
-        <f>D16/A16</f>
+        <f t="shared" si="0"/>
         <v>8.4210827962423614E-4</v>
       </c>
     </row>
@@ -5555,7 +6618,7 @@
         <v>3.5836021332918258E-2</v>
       </c>
       <c r="E17" s="2">
-        <f>D17/A17</f>
+        <f t="shared" si="0"/>
         <v>4.4795026666147823E-3</v>
       </c>
     </row>

</xml_diff>